<commit_message>
Fixed ambigous street type checking. Updated docs.
</commit_message>
<xml_diff>
--- a/Documentation/Address Data Definitions.xlsx
+++ b/Documentation/Address Data Definitions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/82cfe7acc6d68563/Documents/github/verify_Australian_Addresses/Documentation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\NT\verifyAddress\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="66" documentId="13_ncr:1_{0FDE4CD1-142A-4231-8B93-59E254660107}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A769E93F-D259-4299-8924-05590ACFD5F0}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{597325D9-D389-497E-A0C9-FE773E72268F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-16320" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="1" xr2:uid="{F16BFEFE-EA39-4345-81AE-FDCA960E7F0D}"/>
+    <workbookView xWindow="-240" yWindow="-16320" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="1" xr2:uid="{F16BFEFE-EA39-4345-81AE-FDCA960E7F0D}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Dictionary" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2132" uniqueCount="1376">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2143" uniqueCount="1384">
   <si>
     <t>Name</t>
   </si>
@@ -3705,12 +3705,6 @@
   </si>
   <si>
     <t>value:set(statePids)</t>
-  </si>
-  <si>
-    <t>(For sources 'G', 'GA' and 'GN' this is a localityPid. For source'A' this is a postcode)</t>
-  </si>
-  <si>
-    <t>(For sources 'G' , 'GS', 'GA', 'GL' and 'GN' this is a localityPid. For sources 'A', 'AS, and 'AL' this is a postcode)</t>
   </si>
   <si>
     <t>(all the states that sharing this postcode)</t>
@@ -4229,6 +4223,36 @@
   </si>
   <si>
     <t>value: compiled regex for search</t>
+  </si>
+  <si>
+    <t>'GN' - a neighbouring localityName from G-NAF,</t>
+  </si>
+  <si>
+    <t>'C' - a community name</t>
+  </si>
+  <si>
+    <t>(For sources 'G' , 'GS', 'GA', 'GL' and 'GN' this is a G-NAF localityPid)</t>
+  </si>
+  <si>
+    <t>(For sources 'A', 'AS, and 'AL' this is a postcode)</t>
+  </si>
+  <si>
+    <t>(For source 'C' this is a comunity localityPid)</t>
+  </si>
+  <si>
+    <t>(For sources 'G', 'GA' and 'GN' this is a G-NAF localityPid. For source'A' this is a postcode. For source 'C' this is a community localityPid)</t>
+  </si>
+  <si>
+    <t>shortTypes</t>
+  </si>
+  <si>
+    <t>streetTypes found in short street names</t>
+  </si>
+  <si>
+    <t>shortTypeKeys</t>
+  </si>
+  <si>
+    <t>All short street keys for streets that have this streetType in the street name</t>
   </si>
 </sst>
 </file>
@@ -4650,10 +4674,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -5124,11 +5144,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA7F614D-1B52-4687-A9E3-720FABE71083}">
-  <dimension ref="A1:Q149"/>
+  <dimension ref="A1:Q155"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A131" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D142" sqref="D142"/>
+      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F99" sqref="F99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -5225,7 +5245,7 @@
         <v>1221</v>
       </c>
       <c r="F9" t="s">
-        <v>1224</v>
+        <v>1222</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -5254,7 +5274,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="D13" t="s">
-        <v>1330</v>
+        <v>1328</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -5275,7 +5295,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="D16" t="s">
-        <v>1225</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.55000000000000004">
@@ -5379,7 +5399,7 @@
         <v>67</v>
       </c>
       <c r="H27" t="s">
-        <v>1222</v>
+        <v>1379</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.55000000000000004">
@@ -5411,7 +5431,7 @@
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
-        <v>1357</v>
+        <v>1355</v>
       </c>
       <c r="B31" t="s">
         <v>18</v>
@@ -5420,7 +5440,7 @@
         <v>21</v>
       </c>
       <c r="F31" t="s">
-        <v>1360</v>
+        <v>1358</v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.55000000000000004">
@@ -5428,12 +5448,12 @@
         <v>20</v>
       </c>
       <c r="D32" t="s">
-        <v>1358</v>
+        <v>1356</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="D33" t="s">
-        <v>1359</v>
+        <v>1357</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -5460,7 +5480,7 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="45" t="s">
-        <v>1278</v>
+        <v>1276</v>
       </c>
       <c r="B37" t="s">
         <v>18</v>
@@ -5477,21 +5497,21 @@
         <v>23</v>
       </c>
       <c r="D38" t="s">
-        <v>1361</v>
+        <v>1359</v>
       </c>
       <c r="E38" t="s">
-        <v>1279</v>
+        <v>1277</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
+        <v>1368</v>
+      </c>
+      <c r="B39" t="s">
+        <v>1369</v>
+      </c>
+      <c r="D39" t="s">
         <v>1370</v>
-      </c>
-      <c r="B39" t="s">
-        <v>1371</v>
-      </c>
-      <c r="D39" t="s">
-        <v>1372</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -5550,7 +5570,7 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="D46" s="50" t="s">
-        <v>1351</v>
+        <v>1349</v>
       </c>
       <c r="E46" s="50"/>
       <c r="F46" s="50"/>
@@ -5565,7 +5585,7 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" t="s">
-        <v>1337</v>
+        <v>1335</v>
       </c>
       <c r="B48" t="s">
         <v>18</v>
@@ -5576,21 +5596,21 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C49" t="s">
-        <v>1338</v>
+        <v>1336</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" t="s">
-        <v>1329</v>
+        <v>1327</v>
       </c>
       <c r="B51" t="s">
-        <v>1364</v>
+        <v>1362</v>
       </c>
       <c r="C51" s="50" t="s">
-        <v>1362</v>
+        <v>1360</v>
       </c>
       <c r="D51" s="50" t="s">
-        <v>1363</v>
+        <v>1361</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -5658,802 +5678,849 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="F62" s="2" t="s">
-        <v>1342</v>
+        <v>1340</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="F63" s="2" t="s">
-        <v>1343</v>
+        <v>1341</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="F64" s="2" t="s">
-        <v>52</v>
+        <v>1374</v>
       </c>
     </row>
     <row r="65" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="E65" t="s">
+      <c r="F65" s="2" t="s">
+        <v>1375</v>
+      </c>
+    </row>
+    <row r="66" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="E66" t="s">
         <v>23</v>
       </c>
-      <c r="F65" t="s">
-        <v>1223</v>
-      </c>
-    </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="D66" s="50" t="s">
+      <c r="F66" t="s">
+        <v>1376</v>
+      </c>
+    </row>
+    <row r="67" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="F67" t="s">
+        <v>1377</v>
+      </c>
+    </row>
+    <row r="68" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="F68" t="s">
+        <v>1378</v>
+      </c>
+    </row>
+    <row r="69" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="D69" s="50" t="s">
         <v>64</v>
       </c>
-      <c r="E66" s="50"/>
-    </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="D67" s="50" t="s">
+      <c r="E69" s="50"/>
+    </row>
+    <row r="70" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="D70" s="50" t="s">
         <v>65</v>
       </c>
-      <c r="E67" s="50" t="s">
-        <v>1350</v>
-      </c>
-    </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A68" t="s">
+      <c r="E70" s="50" t="s">
+        <v>1348</v>
+      </c>
+    </row>
+    <row r="71" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A71" t="s">
+        <v>1224</v>
+      </c>
+      <c r="B71" t="s">
+        <v>80</v>
+      </c>
+      <c r="C71" t="s">
+        <v>1225</v>
+      </c>
+    </row>
+    <row r="72" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A72" s="41" t="s">
+        <v>87</v>
+      </c>
+      <c r="B72" t="s">
+        <v>80</v>
+      </c>
+      <c r="C72" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="74" spans="1:16" ht="13.8" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A74" s="45" t="s">
+        <v>1278</v>
+      </c>
+      <c r="B74" t="s">
+        <v>18</v>
+      </c>
+      <c r="C74" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="75" spans="1:16" ht="13.8" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="C75" t="s">
+        <v>1213</v>
+      </c>
+      <c r="D75" t="s">
+        <v>1279</v>
+      </c>
+    </row>
+    <row r="76" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A76" s="45" t="s">
+        <v>30</v>
+      </c>
+      <c r="B76" t="s">
+        <v>18</v>
+      </c>
+      <c r="C76" t="s">
+        <v>31</v>
+      </c>
+      <c r="D76" t="s">
+        <v>33</v>
+      </c>
+      <c r="F76" s="43" t="s">
+        <v>1231</v>
+      </c>
+      <c r="J76" s="39" t="s">
         <v>1226</v>
       </c>
-      <c r="B68" t="s">
-        <v>80</v>
-      </c>
-      <c r="C68" t="s">
-        <v>1227</v>
-      </c>
-    </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A69" s="41" t="s">
-        <v>87</v>
-      </c>
-      <c r="B69" t="s">
-        <v>80</v>
-      </c>
-      <c r="C69" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="71" spans="1:16" ht="13.8" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A71" s="45" t="s">
-        <v>1280</v>
-      </c>
-      <c r="B71" t="s">
-        <v>18</v>
-      </c>
-      <c r="C71" t="s">
+      <c r="K76" s="39"/>
+      <c r="L76" s="39"/>
+      <c r="M76" s="39"/>
+      <c r="N76" s="39"/>
+      <c r="O76" s="39"/>
+      <c r="P76" s="39"/>
+    </row>
+    <row r="77" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="C77" t="s">
+        <v>20</v>
+      </c>
+      <c r="D77" t="s">
+        <v>1150</v>
+      </c>
+      <c r="E77" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="78" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="D78" t="s">
+        <v>20</v>
+      </c>
+      <c r="E78" t="s">
+        <v>22</v>
+      </c>
+      <c r="F78" s="45" t="s">
+        <v>1146</v>
+      </c>
+    </row>
+    <row r="79" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="F79" s="46" t="s">
+        <v>1147</v>
+      </c>
+    </row>
+    <row r="80" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="E80" t="s">
+        <v>20</v>
+      </c>
+      <c r="F80" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="72" spans="1:16" ht="13.8" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C72" t="s">
-        <v>1213</v>
-      </c>
-      <c r="D72" t="s">
-        <v>1281</v>
-      </c>
-    </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A73" s="45" t="s">
-        <v>30</v>
-      </c>
-      <c r="B73" t="s">
-        <v>18</v>
-      </c>
-      <c r="C73" t="s">
-        <v>31</v>
-      </c>
-      <c r="D73" t="s">
-        <v>33</v>
-      </c>
-      <c r="F73" s="43" t="s">
-        <v>1233</v>
-      </c>
-      <c r="J73" s="39" t="s">
-        <v>1228</v>
-      </c>
-      <c r="K73" s="39"/>
-      <c r="L73" s="39"/>
-      <c r="M73" s="39"/>
-      <c r="N73" s="39"/>
-      <c r="O73" s="39"/>
-      <c r="P73" s="39"/>
-    </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="C74" t="s">
-        <v>20</v>
-      </c>
-      <c r="D74" t="s">
-        <v>1150</v>
-      </c>
-      <c r="E74" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="D75" t="s">
-        <v>20</v>
-      </c>
-      <c r="E75" t="s">
-        <v>22</v>
-      </c>
-      <c r="F75" s="45" t="s">
-        <v>1146</v>
-      </c>
-    </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="F76" s="46" t="s">
-        <v>1147</v>
-      </c>
-    </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="E77" t="s">
-        <v>20</v>
-      </c>
-      <c r="F77" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="F78" t="s">
+    <row r="81" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="F81" t="s">
         <v>65</v>
       </c>
-      <c r="G78" t="s">
+      <c r="G81" t="s">
         <v>66</v>
-      </c>
-    </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A79" t="s">
-        <v>32</v>
-      </c>
-      <c r="B79" t="s">
-        <v>80</v>
-      </c>
-      <c r="C79" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A80" t="s">
-        <v>111</v>
-      </c>
-      <c r="B80" t="s">
-        <v>80</v>
-      </c>
-      <c r="C80" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A81" t="s">
-        <v>34</v>
-      </c>
-      <c r="B81" t="s">
-        <v>80</v>
-      </c>
-      <c r="C81" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="82" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B82" t="s">
         <v>80</v>
       </c>
       <c r="C82" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="83" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" t="s">
-        <v>1149</v>
+        <v>111</v>
       </c>
       <c r="B83" t="s">
         <v>80</v>
       </c>
       <c r="C83" t="s">
-        <v>1344</v>
-      </c>
-      <c r="F83" s="2"/>
+        <v>95</v>
+      </c>
     </row>
     <row r="84" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" t="s">
+        <v>34</v>
+      </c>
+      <c r="B84" t="s">
+        <v>80</v>
+      </c>
+      <c r="C84" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="85" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A85" t="s">
+        <v>35</v>
+      </c>
+      <c r="B85" t="s">
+        <v>80</v>
+      </c>
+      <c r="C85" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="86" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A86" t="s">
+        <v>1149</v>
+      </c>
+      <c r="B86" t="s">
+        <v>80</v>
+      </c>
+      <c r="C86" t="s">
+        <v>1342</v>
+      </c>
+      <c r="F86" s="2"/>
+    </row>
+    <row r="87" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A87" t="s">
+        <v>1238</v>
+      </c>
+      <c r="B87" t="s">
+        <v>1239</v>
+      </c>
+      <c r="C87" t="s">
         <v>1240</v>
       </c>
-      <c r="B84" t="s">
+      <c r="E87" t="s">
         <v>1241</v>
       </c>
-      <c r="C84" t="s">
-        <v>1242</v>
-      </c>
-      <c r="E84" t="s">
-        <v>1243</v>
-      </c>
-      <c r="F84" s="2"/>
-    </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="F85" s="2"/>
-    </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A86" s="45" t="s">
+      <c r="F87" s="2"/>
+    </row>
+    <row r="88" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="F88" s="2"/>
+    </row>
+    <row r="89" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A89" s="45" t="s">
         <v>96</v>
       </c>
-      <c r="B86" t="s">
+      <c r="B89" t="s">
         <v>18</v>
       </c>
-      <c r="C86" t="s">
+      <c r="C89" t="s">
         <v>1208</v>
       </c>
-      <c r="E86" t="s">
+      <c r="E89" t="s">
         <v>1148</v>
       </c>
-      <c r="J86" s="39" t="s">
-        <v>1229</v>
-      </c>
-      <c r="K86" s="39"/>
-      <c r="L86" s="39"/>
-      <c r="M86" s="39"/>
-      <c r="N86" s="39"/>
-      <c r="O86" s="39"/>
-    </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="C87" t="s">
+      <c r="J89" s="39" t="s">
+        <v>1227</v>
+      </c>
+      <c r="K89" s="39"/>
+      <c r="L89" s="39"/>
+      <c r="M89" s="39"/>
+      <c r="N89" s="39"/>
+      <c r="O89" s="39"/>
+    </row>
+    <row r="90" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="C90" t="s">
         <v>20</v>
       </c>
-      <c r="D87" t="s">
+      <c r="D90" t="s">
         <v>22</v>
       </c>
-      <c r="E87" s="45" t="s">
+      <c r="E90" s="45" t="s">
         <v>1146</v>
       </c>
     </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="E88" s="46" t="s">
+    <row r="91" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="E91" s="46" t="s">
         <v>1147</v>
       </c>
     </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="D89" t="s">
+    <row r="92" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="D92" t="s">
         <v>20</v>
       </c>
-      <c r="E89" s="2" t="s">
+      <c r="E92" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="E90" t="s">
+    <row r="93" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="E93" t="s">
         <v>65</v>
       </c>
-      <c r="F90" t="s">
+      <c r="F93" t="s">
         <v>66</v>
-      </c>
-    </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="D91" s="50" t="s">
-        <v>1335</v>
-      </c>
-    </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="D92" s="50" t="s">
-        <v>1336</v>
-      </c>
-    </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="D93" s="50" t="s">
-        <v>1209</v>
       </c>
     </row>
     <row r="94" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="D94" s="50" t="s">
+        <v>1333</v>
+      </c>
+    </row>
+    <row r="95" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="D95" s="50" t="s">
+        <v>1334</v>
+      </c>
+    </row>
+    <row r="96" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="D96" s="50" t="s">
+        <v>1209</v>
+      </c>
+    </row>
+    <row r="97" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="D97" s="50" t="s">
         <v>1210</v>
       </c>
     </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A95" s="45" t="s">
-        <v>1238</v>
-      </c>
-      <c r="B95" t="s">
+    <row r="98" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A98" t="s">
+        <v>1380</v>
+      </c>
+      <c r="B98" t="s">
+        <v>1369</v>
+      </c>
+      <c r="C98" t="s">
+        <v>1381</v>
+      </c>
+      <c r="D98" s="50"/>
+    </row>
+    <row r="99" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A99" t="s">
+        <v>1382</v>
+      </c>
+      <c r="B99" t="s">
         <v>18</v>
       </c>
-      <c r="C95" t="s">
-        <v>1239</v>
-      </c>
-    </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="C96" t="s">
+      <c r="C99" t="s">
+        <v>70</v>
+      </c>
+      <c r="D99" s="50"/>
+    </row>
+    <row r="100" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="C100" t="s">
+        <v>23</v>
+      </c>
+      <c r="D100" s="50" t="s">
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="101" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A101" s="45" t="s">
+        <v>1236</v>
+      </c>
+      <c r="B101" t="s">
+        <v>18</v>
+      </c>
+      <c r="C101" t="s">
+        <v>1237</v>
+      </c>
+    </row>
+    <row r="102" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="C102" t="s">
         <v>1213</v>
       </c>
-      <c r="D96" t="s">
-        <v>1339</v>
-      </c>
-    </row>
-    <row r="97" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="F97" s="2"/>
-    </row>
-    <row r="98" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A98" s="45" t="s">
+      <c r="D102" t="s">
+        <v>1337</v>
+      </c>
+    </row>
+    <row r="103" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="F103" s="2"/>
+    </row>
+    <row r="104" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A104" s="45" t="s">
         <v>46</v>
       </c>
-      <c r="B98" t="s">
+      <c r="B104" t="s">
         <v>18</v>
       </c>
-      <c r="C98" t="s">
+      <c r="C104" t="s">
         <v>47</v>
       </c>
-      <c r="E98" s="39" t="s">
+      <c r="E104" s="39" t="s">
         <v>1160</v>
       </c>
-      <c r="F98" s="39"/>
-      <c r="G98" s="39"/>
-      <c r="H98" s="39"/>
-      <c r="I98" s="39"/>
-      <c r="J98" s="39"/>
-      <c r="K98" s="39"/>
-      <c r="L98" s="39"/>
-      <c r="M98" s="39"/>
-      <c r="N98" s="39"/>
-      <c r="O98" s="39"/>
-      <c r="P98" s="39"/>
-    </row>
-    <row r="99" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="C99" t="s">
+      <c r="F104" s="39"/>
+      <c r="G104" s="39"/>
+      <c r="H104" s="39"/>
+      <c r="I104" s="39"/>
+      <c r="J104" s="39"/>
+      <c r="K104" s="39"/>
+      <c r="L104" s="39"/>
+      <c r="M104" s="39"/>
+      <c r="N104" s="39"/>
+      <c r="O104" s="39"/>
+      <c r="P104" s="39"/>
+    </row>
+    <row r="105" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="C105" t="s">
         <v>20</v>
       </c>
-      <c r="D99" t="s">
+      <c r="D105" t="s">
         <v>114</v>
       </c>
-      <c r="E99" t="s">
+      <c r="E105" t="s">
         <v>57</v>
       </c>
-      <c r="N99" t="s">
+      <c r="N105" t="s">
         <v>1130</v>
       </c>
     </row>
-    <row r="100" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="D100" t="s">
+    <row r="106" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="D106" t="s">
         <v>65</v>
       </c>
-      <c r="E100" t="s">
-        <v>1244</v>
-      </c>
-      <c r="I100" t="s">
+      <c r="E106" t="s">
+        <v>1242</v>
+      </c>
+      <c r="I106" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="101" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="I101" t="s">
+    <row r="107" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="I107" t="s">
         <v>1145</v>
       </c>
     </row>
-    <row r="102" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="I102" t="s">
+    <row r="108" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="I108" t="s">
         <v>1131</v>
       </c>
     </row>
-    <row r="103" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="I103" t="s">
+    <row r="109" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="I109" t="s">
         <v>1132</v>
       </c>
     </row>
-    <row r="104" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="E104" t="s">
+    <row r="110" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="E110" t="s">
         <v>116</v>
-      </c>
-    </row>
-    <row r="105" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="E105" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="106" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A106" t="s">
-        <v>112</v>
-      </c>
-      <c r="B106" t="s">
-        <v>1345</v>
-      </c>
-      <c r="C106" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="107" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A107" s="41" t="s">
-        <v>1328</v>
-      </c>
-      <c r="B107" t="s">
-        <v>1345</v>
-      </c>
-      <c r="C107" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="109" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A109" t="s">
-        <v>68</v>
-      </c>
-      <c r="B109" t="s">
-        <v>18</v>
-      </c>
-      <c r="C109" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="110" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="C110" t="s">
-        <v>65</v>
-      </c>
-      <c r="D110" t="s">
-        <v>1138</v>
-      </c>
-      <c r="K110" s="2" t="s">
-        <v>1218</v>
       </c>
     </row>
     <row r="111" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="E111" t="s">
-        <v>1139</v>
-      </c>
-      <c r="J111" s="2"/>
+        <v>115</v>
+      </c>
     </row>
     <row r="112" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A112" t="s">
-        <v>1352</v>
+        <v>112</v>
       </c>
       <c r="B112" t="s">
+        <v>1343</v>
+      </c>
+      <c r="C112" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="113" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A113" s="41" t="s">
+        <v>1326</v>
+      </c>
+      <c r="B113" t="s">
+        <v>1343</v>
+      </c>
+      <c r="C113" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="115" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A115" t="s">
+        <v>68</v>
+      </c>
+      <c r="B115" t="s">
         <v>18</v>
       </c>
-      <c r="C112" t="s">
+      <c r="C115" t="s">
         <v>70</v>
       </c>
-      <c r="J112" s="2"/>
-    </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="C113" t="s">
-        <v>1353</v>
-      </c>
-      <c r="J113" s="2"/>
-    </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A114" t="s">
-        <v>1354</v>
-      </c>
-      <c r="B114" t="s">
-        <v>18</v>
-      </c>
-      <c r="C114" t="s">
-        <v>70</v>
-      </c>
-      <c r="J114" s="2"/>
-    </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="C115" t="s">
-        <v>1355</v>
-      </c>
-      <c r="D115" t="s">
-        <v>1356</v>
-      </c>
-      <c r="J115" s="2"/>
-    </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A116" t="s">
-        <v>1235</v>
-      </c>
-      <c r="B116" t="s">
-        <v>18</v>
-      </c>
+    </row>
+    <row r="116" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="C116" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="C117" t="s">
         <v>65</v>
       </c>
-      <c r="D117" t="s">
-        <v>76</v>
-      </c>
-      <c r="G117" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A118" s="45" t="s">
-        <v>97</v>
+      <c r="D116" t="s">
+        <v>1138</v>
+      </c>
+      <c r="K116" s="2" t="s">
+        <v>1218</v>
+      </c>
+    </row>
+    <row r="117" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="E117" t="s">
+        <v>1139</v>
+      </c>
+      <c r="J117" s="2"/>
+    </row>
+    <row r="118" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A118" t="s">
+        <v>1350</v>
       </c>
       <c r="B118" t="s">
         <v>18</v>
       </c>
       <c r="C118" t="s">
-        <v>61</v>
-      </c>
-      <c r="D118" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+        <v>70</v>
+      </c>
+      <c r="J118" s="2"/>
+    </row>
+    <row r="119" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="C119" t="s">
-        <v>98</v>
-      </c>
-      <c r="D119" t="s">
-        <v>1230</v>
-      </c>
-    </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+        <v>1351</v>
+      </c>
+      <c r="J119" s="2"/>
+    </row>
+    <row r="120" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A120" t="s">
-        <v>1231</v>
+        <v>1352</v>
       </c>
       <c r="B120" t="s">
         <v>18</v>
       </c>
       <c r="C120" t="s">
-        <v>47</v>
-      </c>
-      <c r="D120" t="s">
-        <v>1230</v>
-      </c>
-    </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+        <v>70</v>
+      </c>
+      <c r="J120" s="2"/>
+    </row>
+    <row r="121" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="C121" t="s">
-        <v>1232</v>
+        <v>1353</v>
       </c>
       <c r="D121" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A122" s="45" t="s">
-        <v>105</v>
+        <v>1354</v>
+      </c>
+      <c r="J121" s="2"/>
+    </row>
+    <row r="122" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A122" t="s">
+        <v>1233</v>
       </c>
       <c r="B122" t="s">
         <v>18</v>
       </c>
       <c r="C122" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="123" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="C123" t="s">
+        <v>65</v>
+      </c>
+      <c r="D123" t="s">
+        <v>76</v>
+      </c>
+      <c r="G123" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="124" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A124" s="45" t="s">
+        <v>97</v>
+      </c>
+      <c r="B124" t="s">
+        <v>18</v>
+      </c>
+      <c r="C124" t="s">
+        <v>61</v>
+      </c>
+      <c r="D124" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="125" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="C125" t="s">
+        <v>98</v>
+      </c>
+      <c r="D125" t="s">
+        <v>1228</v>
+      </c>
+    </row>
+    <row r="126" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A126" t="s">
+        <v>1229</v>
+      </c>
+      <c r="B126" t="s">
+        <v>18</v>
+      </c>
+      <c r="C126" t="s">
+        <v>47</v>
+      </c>
+      <c r="D126" t="s">
+        <v>1228</v>
+      </c>
+    </row>
+    <row r="127" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="C127" t="s">
+        <v>1230</v>
+      </c>
+      <c r="D127" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="128" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A128" s="45" t="s">
+        <v>105</v>
+      </c>
+      <c r="B128" t="s">
+        <v>18</v>
+      </c>
+      <c r="C128" t="s">
         <v>24</v>
       </c>
-      <c r="D122" t="s">
+      <c r="D128" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="C123" t="s">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C129" t="s">
         <v>98</v>
       </c>
-      <c r="D123" t="s">
-        <v>1230</v>
-      </c>
-    </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A125" t="s">
+      <c r="D129" t="s">
+        <v>1228</v>
+      </c>
+    </row>
+    <row r="131" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A131" t="s">
         <v>94</v>
       </c>
-      <c r="B125" t="s">
+      <c r="B131" t="s">
         <v>18</v>
       </c>
-      <c r="C125" t="s">
+      <c r="C131" t="s">
         <v>1150</v>
       </c>
     </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="C126" t="s">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C132" t="s">
         <v>20</v>
       </c>
-      <c r="D126" t="s">
+      <c r="D132" t="s">
         <v>22</v>
       </c>
-      <c r="E126" t="s">
+      <c r="E132" t="s">
         <v>1146</v>
       </c>
     </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="E127" s="2" t="s">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="E133" s="2" t="s">
         <v>1147</v>
       </c>
     </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="E128" s="2" t="s">
-        <v>1236</v>
-      </c>
-    </row>
-    <row r="129" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="E129" s="2" t="s">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="E134" s="2" t="s">
         <v>1234</v>
       </c>
     </row>
-    <row r="130" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="E130" s="2" t="s">
-        <v>1340</v>
-      </c>
-    </row>
-    <row r="131" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="E131" s="2" t="s">
-        <v>1341</v>
-      </c>
-    </row>
-    <row r="132" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="D132" t="s">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="E135" s="2" t="s">
+        <v>1232</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="E136" s="2" t="s">
+        <v>1338</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="E137" s="2" t="s">
+        <v>1339</v>
+      </c>
+    </row>
+    <row r="138" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="D138" t="s">
         <v>20</v>
       </c>
-      <c r="E132" s="2" t="s">
+      <c r="E138" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="133" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="E133" t="s">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="E139" t="s">
         <v>65</v>
       </c>
-      <c r="F133" t="s">
+      <c r="F139" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="134" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="D134" t="s">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="D140" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="135" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="D135" t="s">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="D141" t="s">
         <v>65</v>
       </c>
-      <c r="E135" t="s">
-        <v>1237</v>
-      </c>
-    </row>
-    <row r="136" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A136" t="s">
+      <c r="E141" t="s">
+        <v>1235</v>
+      </c>
+    </row>
+    <row r="142" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A142" t="s">
         <v>107</v>
       </c>
-      <c r="B136" t="s">
+      <c r="B142" t="s">
+        <v>1329</v>
+      </c>
+      <c r="C142" t="s">
+        <v>1330</v>
+      </c>
+      <c r="D142" t="s">
+        <v>1332</v>
+      </c>
+      <c r="E142" t="s">
         <v>1331</v>
       </c>
-      <c r="C136" t="s">
-        <v>1332</v>
-      </c>
-      <c r="D136" t="s">
-        <v>1334</v>
-      </c>
-      <c r="E136" t="s">
-        <v>1333</v>
-      </c>
-    </row>
-    <row r="138" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A138" s="45" t="s">
+    </row>
+    <row r="144" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A144" s="45" t="s">
         <v>38</v>
       </c>
-      <c r="B138" t="s">
+      <c r="B144" t="s">
         <v>18</v>
       </c>
-      <c r="C138" t="s">
+      <c r="C144" t="s">
         <v>1133</v>
       </c>
-      <c r="E138" s="39" t="s">
+      <c r="E144" s="39" t="s">
         <v>1161</v>
       </c>
-      <c r="F138" s="39"/>
-      <c r="G138" s="39"/>
-      <c r="H138" s="39"/>
-    </row>
-    <row r="139" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="C139" s="50" t="s">
+      <c r="F144" s="39"/>
+      <c r="G144" s="39"/>
+      <c r="H144" s="39"/>
+    </row>
+    <row r="145" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="C145" s="50" t="s">
         <v>65</v>
       </c>
-      <c r="D139" s="50" t="s">
-        <v>1365</v>
-      </c>
-    </row>
-    <row r="140" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A140" t="s">
+      <c r="D145" s="50" t="s">
+        <v>1363</v>
+      </c>
+    </row>
+    <row r="146" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A146" t="s">
+        <v>1371</v>
+      </c>
+      <c r="B146" t="s">
+        <v>18</v>
+      </c>
+      <c r="C146" s="50" t="s">
+        <v>1372</v>
+      </c>
+      <c r="D146" s="50"/>
+    </row>
+    <row r="147" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="C147" s="50" t="s">
         <v>1373</v>
       </c>
-      <c r="B140" t="s">
-        <v>18</v>
-      </c>
-      <c r="C140" s="50" t="s">
-        <v>1374</v>
-      </c>
-      <c r="D140" s="50"/>
-    </row>
-    <row r="141" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="C141" s="50" t="s">
-        <v>1375</v>
-      </c>
-      <c r="D141" s="50"/>
-    </row>
-    <row r="142" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A142" t="s">
+      <c r="D147" s="50"/>
+    </row>
+    <row r="148" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A148" t="s">
         <v>1134</v>
-      </c>
-      <c r="B142" t="s">
-        <v>1140</v>
-      </c>
-      <c r="C142" t="s">
-        <v>1215</v>
-      </c>
-      <c r="E142" t="s">
-        <v>1317</v>
-      </c>
-      <c r="M142" t="s">
-        <v>1321</v>
-      </c>
-    </row>
-    <row r="143" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="E143" t="s">
-        <v>1318</v>
-      </c>
-      <c r="M143" t="s">
-        <v>1322</v>
-      </c>
-    </row>
-    <row r="144" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A144" t="s">
-        <v>1135</v>
-      </c>
-      <c r="B144" t="s">
-        <v>1140</v>
-      </c>
-      <c r="C144" t="s">
-        <v>1215</v>
-      </c>
-      <c r="E144" t="s">
-        <v>1216</v>
-      </c>
-      <c r="M144" t="s">
-        <v>1321</v>
-      </c>
-    </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A145" t="s">
-        <v>1217</v>
-      </c>
-      <c r="B145" t="s">
-        <v>1214</v>
-      </c>
-      <c r="C145" t="s">
-        <v>1215</v>
-      </c>
-      <c r="E145" t="s">
-        <v>1219</v>
-      </c>
-    </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A146" t="s">
-        <v>1141</v>
-      </c>
-      <c r="B146" t="s">
-        <v>1140</v>
-      </c>
-      <c r="C146" t="s">
-        <v>1143</v>
-      </c>
-      <c r="E146" t="s">
-        <v>1144</v>
-      </c>
-    </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A148" t="s">
-        <v>1369</v>
       </c>
       <c r="B148" t="s">
         <v>1140</v>
       </c>
       <c r="C148" t="s">
+        <v>1215</v>
+      </c>
+      <c r="E148" t="s">
+        <v>1315</v>
+      </c>
+      <c r="M148" t="s">
+        <v>1319</v>
+      </c>
+    </row>
+    <row r="149" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="E149" t="s">
+        <v>1316</v>
+      </c>
+      <c r="M149" t="s">
+        <v>1320</v>
+      </c>
+    </row>
+    <row r="150" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A150" t="s">
+        <v>1135</v>
+      </c>
+      <c r="B150" t="s">
+        <v>1140</v>
+      </c>
+      <c r="C150" t="s">
+        <v>1215</v>
+      </c>
+      <c r="E150" t="s">
+        <v>1216</v>
+      </c>
+      <c r="M150" t="s">
+        <v>1319</v>
+      </c>
+    </row>
+    <row r="151" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A151" t="s">
+        <v>1217</v>
+      </c>
+      <c r="B151" t="s">
+        <v>1214</v>
+      </c>
+      <c r="C151" t="s">
+        <v>1215</v>
+      </c>
+      <c r="E151" t="s">
+        <v>1219</v>
+      </c>
+    </row>
+    <row r="152" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A152" t="s">
+        <v>1141</v>
+      </c>
+      <c r="B152" t="s">
+        <v>1140</v>
+      </c>
+      <c r="C152" t="s">
+        <v>1143</v>
+      </c>
+      <c r="E152" t="s">
+        <v>1144</v>
+      </c>
+    </row>
+    <row r="154" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A154" t="s">
+        <v>1367</v>
+      </c>
+      <c r="B154" t="s">
+        <v>1140</v>
+      </c>
+      <c r="C154" t="s">
         <v>1133</v>
       </c>
-      <c r="F148" t="s">
+      <c r="F154" t="s">
+        <v>1364</v>
+      </c>
+    </row>
+    <row r="155" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="C155" s="50" t="s">
+        <v>65</v>
+      </c>
+      <c r="D155" s="50" t="s">
         <v>1366</v>
       </c>
-    </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="C149" s="50" t="s">
-        <v>65</v>
-      </c>
-      <c r="D149" s="50" t="s">
-        <v>1368</v>
-      </c>
-      <c r="F149" t="s">
-        <v>1367</v>
+      <c r="F155" t="s">
+        <v>1365</v>
       </c>
     </row>
   </sheetData>
@@ -6716,27 +6783,27 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="D48" t="s">
-        <v>1306</v>
+        <v>1304</v>
       </c>
     </row>
     <row r="49" spans="4:5" x14ac:dyDescent="0.55000000000000004">
       <c r="E49" t="s">
-        <v>1307</v>
+        <v>1305</v>
       </c>
     </row>
     <row r="50" spans="4:5" x14ac:dyDescent="0.55000000000000004">
       <c r="E50" t="s">
-        <v>1308</v>
+        <v>1306</v>
       </c>
     </row>
     <row r="52" spans="4:5" x14ac:dyDescent="0.55000000000000004">
       <c r="D52" t="s">
-        <v>1309</v>
+        <v>1307</v>
       </c>
     </row>
     <row r="53" spans="4:5" x14ac:dyDescent="0.55000000000000004">
       <c r="E53" t="s">
-        <v>1310</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="54" spans="4:5" x14ac:dyDescent="0.55000000000000004">
@@ -6969,7 +7036,7 @@
         <v>136</v>
       </c>
       <c r="M11" t="s">
-        <v>1323</v>
+        <v>1321</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -7001,7 +7068,7 @@
         <v>588</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>1324</v>
+        <v>1322</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -7033,7 +7100,7 @@
         <v>564</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>1324</v>
+        <v>1322</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -7059,7 +7126,7 @@
         <v>566</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>1325</v>
+        <v>1323</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -7091,7 +7158,7 @@
         <v>568</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -7129,7 +7196,7 @@
         <v>570</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -7167,7 +7234,7 @@
         <v>572</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -7205,7 +7272,7 @@
         <v>574</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -7240,7 +7307,7 @@
         <v>576</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -7275,7 +7342,7 @@
         <v>578</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -7307,7 +7374,7 @@
         <v>580</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -7339,7 +7406,7 @@
         <v>582</v>
       </c>
       <c r="M22" s="2" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -7388,10 +7455,10 @@
         <v>174</v>
       </c>
       <c r="K24" s="44" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
       <c r="M24" s="2" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -7417,13 +7484,13 @@
         <v>176</v>
       </c>
       <c r="K25" s="44" t="s">
-        <v>1250</v>
+        <v>1248</v>
       </c>
       <c r="L25" s="44" t="s">
-        <v>1251</v>
+        <v>1249</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -7449,10 +7516,10 @@
         <v>178</v>
       </c>
       <c r="K26" s="44" t="s">
-        <v>1326</v>
+        <v>1324</v>
       </c>
       <c r="M26" s="2" t="s">
-        <v>1324</v>
+        <v>1322</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -12583,23 +12650,23 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>1346</v>
+        <v>1344</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>1319</v>
+        <v>1317</v>
       </c>
       <c r="B14" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
-        <v>1320</v>
+        <v>1318</v>
       </c>
       <c r="B15" t="s">
-        <v>1348</v>
+        <v>1346</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -12607,7 +12674,7 @@
         <v>1207</v>
       </c>
       <c r="B16" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
     </row>
   </sheetData>
@@ -12633,133 +12700,133 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>1245</v>
+        <v>1243</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>1246</v>
+        <v>1244</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>1260</v>
+        <v>1258</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>1247</v>
+        <v>1245</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="B5" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="B6" t="s">
-        <v>1252</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>1264</v>
+        <v>1262</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>1253</v>
+        <v>1251</v>
       </c>
       <c r="B9" t="s">
-        <v>1254</v>
+        <v>1252</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>1255</v>
+        <v>1253</v>
       </c>
       <c r="B10" t="s">
-        <v>1256</v>
+        <v>1254</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="B11" t="s">
-        <v>1257</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="C13" t="s">
-        <v>1265</v>
+        <v>1263</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="C14" t="s">
-        <v>1259</v>
+        <v>1257</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="C16" t="s">
-        <v>1261</v>
+        <v>1259</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="C17" t="s">
-        <v>1262</v>
+        <v>1260</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="C18" t="s">
-        <v>1263</v>
+        <v>1261</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="C19" t="s">
-        <v>1266</v>
+        <v>1264</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="C20" t="s">
-        <v>1267</v>
+        <v>1265</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="C22" t="s">
-        <v>1269</v>
+        <v>1267</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="C23" t="s">
-        <v>1268</v>
+        <v>1266</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
-        <v>1270</v>
+        <v>1268</v>
       </c>
       <c r="C25" t="s">
-        <v>1271</v>
+        <v>1269</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="C26" t="s">
-        <v>1272</v>
+        <v>1270</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B28" s="47" t="s">
-        <v>1282</v>
+        <v>1280</v>
       </c>
       <c r="C28" s="47" t="s">
-        <v>1273</v>
+        <v>1271</v>
       </c>
       <c r="D28" s="47" t="s">
-        <v>1295</v>
+        <v>1293</v>
       </c>
       <c r="E28" s="47" t="s">
-        <v>1274</v>
+        <v>1272</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -12767,13 +12834,13 @@
         <v>62</v>
       </c>
       <c r="C29" s="47" t="s">
+        <v>1273</v>
+      </c>
+      <c r="D29" s="47" t="s">
+        <v>1274</v>
+      </c>
+      <c r="E29" s="47" t="s">
         <v>1275</v>
-      </c>
-      <c r="D29" s="47" t="s">
-        <v>1276</v>
-      </c>
-      <c r="E29" s="47" t="s">
-        <v>1277</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -12781,16 +12848,16 @@
         <v>59</v>
       </c>
       <c r="C30" s="57" t="s">
-        <v>1284</v>
+        <v>1282</v>
       </c>
       <c r="D30" s="57"/>
       <c r="E30" s="57" t="s">
-        <v>1286</v>
+        <v>1284</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B31" s="47" t="s">
-        <v>1297</v>
+        <v>1295</v>
       </c>
       <c r="C31" s="57"/>
       <c r="D31" s="57"/>
@@ -12809,18 +12876,18 @@
         <v>89</v>
       </c>
       <c r="C33" s="51" t="s">
-        <v>1293</v>
+        <v>1291</v>
       </c>
       <c r="D33" s="51" t="s">
-        <v>1294</v>
+        <v>1292</v>
       </c>
       <c r="E33" s="54" t="s">
-        <v>1283</v>
+        <v>1281</v>
       </c>
     </row>
     <row r="34" spans="2:5" ht="16.5" x14ac:dyDescent="0.55000000000000004">
       <c r="B34" s="47" t="s">
-        <v>1299</v>
+        <v>1297</v>
       </c>
       <c r="C34" s="52"/>
       <c r="D34" s="52"/>
@@ -12828,7 +12895,7 @@
     </row>
     <row r="35" spans="2:5" ht="16.5" x14ac:dyDescent="0.55000000000000004">
       <c r="B35" s="47" t="s">
-        <v>1298</v>
+        <v>1296</v>
       </c>
       <c r="C35" s="53"/>
       <c r="D35" s="53"/>
@@ -12836,14 +12903,14 @@
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B36" s="47" t="s">
+        <v>1283</v>
+      </c>
+      <c r="C36" s="54" t="s">
         <v>1285</v>
-      </c>
-      <c r="C36" s="54" t="s">
-        <v>1287</v>
       </c>
       <c r="D36" s="54"/>
       <c r="E36" s="54" t="s">
-        <v>1288</v>
+        <v>1286</v>
       </c>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.55000000000000004">
@@ -12856,16 +12923,16 @@
     </row>
     <row r="38" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B38" s="47" t="s">
-        <v>1280</v>
+        <v>1278</v>
       </c>
       <c r="C38" s="51" t="s">
-        <v>1291</v>
+        <v>1289</v>
       </c>
       <c r="D38" s="51" t="s">
-        <v>1292</v>
+        <v>1290</v>
       </c>
       <c r="E38" s="54" t="s">
-        <v>1289</v>
+        <v>1287</v>
       </c>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.55000000000000004">
@@ -12886,59 +12953,59 @@
     </row>
     <row r="41" spans="2:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="B41" s="49" t="s">
-        <v>1296</v>
+        <v>1294</v>
       </c>
       <c r="C41" s="47" t="s">
-        <v>1301</v>
+        <v>1299</v>
       </c>
       <c r="D41" s="47"/>
       <c r="E41" s="47" t="s">
-        <v>1290</v>
+        <v>1288</v>
       </c>
     </row>
     <row r="42" spans="2:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="B42" s="49" t="s">
+        <v>1300</v>
+      </c>
+      <c r="C42" s="49" t="s">
+        <v>1301</v>
+      </c>
+      <c r="D42" s="49" t="s">
+        <v>1303</v>
+      </c>
+      <c r="E42" s="49" t="s">
         <v>1302</v>
-      </c>
-      <c r="C42" s="49" t="s">
-        <v>1303</v>
-      </c>
-      <c r="D42" s="49" t="s">
-        <v>1305</v>
-      </c>
-      <c r="E42" s="49" t="s">
-        <v>1304</v>
       </c>
     </row>
     <row r="43" spans="2:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="B43" s="47" t="s">
+        <v>1309</v>
+      </c>
+      <c r="C43" s="48" t="s">
+        <v>1310</v>
+      </c>
+      <c r="D43" s="48" t="s">
         <v>1311</v>
       </c>
-      <c r="C43" s="48" t="s">
+      <c r="E43" s="48" t="s">
         <v>1312</v>
-      </c>
-      <c r="D43" s="48" t="s">
-        <v>1313</v>
-      </c>
-      <c r="E43" s="48" t="s">
-        <v>1314</v>
       </c>
     </row>
     <row r="44" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B44" s="47" t="s">
-        <v>1315</v>
+        <v>1313</v>
       </c>
       <c r="C44" s="37" t="s">
-        <v>1315</v>
+        <v>1313</v>
       </c>
       <c r="D44" s="37"/>
       <c r="E44" s="37" t="s">
-        <v>1316</v>
+        <v>1314</v>
       </c>
     </row>
     <row r="48" spans="2:5" ht="16.5" x14ac:dyDescent="0.55000000000000004">
       <c r="B48" t="s">
-        <v>1300</v>
+        <v>1298</v>
       </c>
     </row>
   </sheetData>

</xml_diff>